<commit_message>
added speficied dates option
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\New folder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\clockify-report-generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F0B9BD6-84CA-4D90-8267-3F0FC553EAC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450"/>
   </bookViews>
   <sheets>
     <sheet name="WAR" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="i4b/1A4qJkJ3cZUWmstGeB0b5YnzUlHJvyWqychGoNo="/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Name:</t>
   </si>
@@ -59,11 +58,14 @@
   <si>
     <t>Overall Total:</t>
   </si>
+  <si>
+    <t>z</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
   </numFmts>
@@ -116,9 +118,7 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -132,7 +132,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="-0.499984740745262"/>
+        <fgColor rgb="FFDBB7FF"/>
         <bgColor rgb="FFFFCCFF"/>
       </patternFill>
     </fill>
@@ -352,8 +352,19 @@
     <xf numFmtId="2" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -364,22 +375,11 @@
     <xf numFmtId="21" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="2" fontId="9" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -388,6 +388,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFDBB7FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -596,62 +601,62 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N1025"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E55" sqref="D55:E55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" customWidth="1"/>
-    <col min="2" max="2" width="62.5546875" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" customWidth="1"/>
-    <col min="7" max="26" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="62.5703125" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" customWidth="1"/>
+    <col min="7" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="14.4">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="37"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="27"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:14" ht="14.4">
+    <row r="2" spans="1:14">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="37"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="27"/>
       <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:14" ht="17.25" customHeight="1">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="35"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
       <c r="F3" s="5"/>
     </row>
-    <row r="4" spans="1:14" ht="14.4">
-      <c r="A4" s="38" t="s">
+    <row r="4" spans="1:14">
+      <c r="A4" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="36"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="37"/>
-    </row>
-    <row r="5" spans="1:14" thickBot="1">
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="27"/>
+    </row>
+    <row r="5" spans="1:14" ht="15.75" thickBot="1">
       <c r="A5" s="6" t="s">
         <v>4</v>
       </c>
@@ -672,14 +677,16 @@
       </c>
     </row>
     <row r="6" spans="1:14" ht="64.5" customHeight="1" thickBot="1">
-      <c r="A6" s="8"/>
+      <c r="A6" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="B6" s="19"/>
       <c r="C6" s="16"/>
       <c r="D6" s="16"/>
       <c r="E6" s="24"/>
       <c r="F6" s="16"/>
     </row>
-    <row r="7" spans="1:14" ht="30.6" customHeight="1" thickBot="1">
+    <row r="7" spans="1:14" ht="30" customHeight="1" thickBot="1">
       <c r="A7" s="8"/>
       <c r="B7" s="7"/>
       <c r="C7" s="16"/>
@@ -711,7 +718,7 @@
       <c r="E10" s="24"/>
       <c r="F10" s="21"/>
     </row>
-    <row r="11" spans="1:14" ht="16.2" customHeight="1" thickBot="1">
+    <row r="11" spans="1:14" ht="16.149999999999999" customHeight="1" thickBot="1">
       <c r="A11" s="8"/>
       <c r="B11" s="7"/>
       <c r="C11" s="16"/>
@@ -719,7 +726,7 @@
       <c r="E11" s="24"/>
       <c r="F11" s="21"/>
     </row>
-    <row r="12" spans="1:14" ht="16.2" customHeight="1" thickBot="1">
+    <row r="12" spans="1:14" ht="16.149999999999999" customHeight="1" thickBot="1">
       <c r="A12" s="8"/>
       <c r="B12" s="7"/>
       <c r="C12" s="16"/>
@@ -727,13 +734,13 @@
       <c r="E12" s="24"/>
       <c r="F12" s="21"/>
     </row>
-    <row r="13" spans="1:14" ht="16.2" thickBot="1">
-      <c r="A13" s="31"/>
-      <c r="B13" s="32"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="33"/>
+    <row r="13" spans="1:14" ht="16.5" thickBot="1">
+      <c r="A13" s="29"/>
+      <c r="B13" s="30"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="31"/>
       <c r="K13" s="10"/>
       <c r="L13" s="11"/>
       <c r="M13" s="12"/>
@@ -779,7 +786,7 @@
       <c r="E18" s="24"/>
       <c r="F18" s="21"/>
     </row>
-    <row r="19" spans="1:14" ht="16.2" customHeight="1" thickBot="1">
+    <row r="19" spans="1:14" ht="16.149999999999999" customHeight="1" thickBot="1">
       <c r="A19" s="8"/>
       <c r="B19" s="7"/>
       <c r="C19" s="16"/>
@@ -787,7 +794,7 @@
       <c r="E19" s="24"/>
       <c r="F19" s="21"/>
     </row>
-    <row r="20" spans="1:14" ht="16.2" customHeight="1" thickBot="1">
+    <row r="20" spans="1:14" ht="16.149999999999999" customHeight="1" thickBot="1">
       <c r="A20" s="8"/>
       <c r="B20" s="7"/>
       <c r="C20" s="16"/>
@@ -795,13 +802,13 @@
       <c r="E20" s="24"/>
       <c r="F20" s="21"/>
     </row>
-    <row r="21" spans="1:14" ht="16.2" thickBot="1">
-      <c r="A21" s="31"/>
-      <c r="B21" s="32"/>
-      <c r="C21" s="33"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="29"/>
-      <c r="F21" s="33"/>
+    <row r="21" spans="1:14" ht="16.5" thickBot="1">
+      <c r="A21" s="29"/>
+      <c r="B21" s="30"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="31"/>
       <c r="K21" s="10"/>
       <c r="L21" s="11"/>
       <c r="M21" s="12"/>
@@ -891,13 +898,13 @@
       <c r="M28" s="12"/>
       <c r="N28" s="12"/>
     </row>
-    <row r="29" spans="1:14" ht="16.2" thickBot="1">
-      <c r="A29" s="31"/>
-      <c r="B29" s="32"/>
-      <c r="C29" s="33"/>
-      <c r="D29" s="33"/>
-      <c r="E29" s="29"/>
-      <c r="F29" s="33"/>
+    <row r="29" spans="1:14" ht="16.5" thickBot="1">
+      <c r="A29" s="29"/>
+      <c r="B29" s="30"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="31"/>
       <c r="K29" s="10"/>
       <c r="L29" s="11"/>
       <c r="M29" s="12"/>
@@ -927,7 +934,7 @@
       <c r="M31" s="12"/>
       <c r="N31" s="12"/>
     </row>
-    <row r="32" spans="1:14" ht="16.2" thickBot="1">
+    <row r="32" spans="1:14" ht="16.5" thickBot="1">
       <c r="A32" s="15"/>
       <c r="B32" s="20"/>
       <c r="C32" s="16"/>
@@ -939,7 +946,7 @@
       <c r="M32" s="12"/>
       <c r="N32" s="12"/>
     </row>
-    <row r="33" spans="1:14" ht="16.2" thickBot="1">
+    <row r="33" spans="1:14" ht="16.5" thickBot="1">
       <c r="A33" s="15"/>
       <c r="B33" s="20"/>
       <c r="C33" s="16"/>
@@ -951,7 +958,7 @@
       <c r="M33" s="12"/>
       <c r="N33" s="12"/>
     </row>
-    <row r="34" spans="1:14" ht="16.2" thickBot="1">
+    <row r="34" spans="1:14" ht="16.5" thickBot="1">
       <c r="A34" s="15"/>
       <c r="B34" s="20"/>
       <c r="C34" s="16"/>
@@ -963,7 +970,7 @@
       <c r="M34" s="12"/>
       <c r="N34" s="12"/>
     </row>
-    <row r="35" spans="1:14" ht="16.2" thickBot="1">
+    <row r="35" spans="1:14" ht="16.5" thickBot="1">
       <c r="A35" s="15"/>
       <c r="B35" s="13"/>
       <c r="C35" s="16"/>
@@ -975,7 +982,7 @@
       <c r="M35" s="12"/>
       <c r="N35" s="12"/>
     </row>
-    <row r="36" spans="1:14" ht="16.2" thickBot="1">
+    <row r="36" spans="1:14" ht="16.5" thickBot="1">
       <c r="A36" s="15"/>
       <c r="B36" s="14"/>
       <c r="C36" s="16"/>
@@ -987,13 +994,13 @@
       <c r="M36" s="12"/>
       <c r="N36" s="12"/>
     </row>
-    <row r="37" spans="1:14" ht="16.2" thickBot="1">
-      <c r="A37" s="31"/>
-      <c r="B37" s="32"/>
-      <c r="C37" s="33"/>
-      <c r="D37" s="33"/>
-      <c r="E37" s="29"/>
-      <c r="F37" s="33"/>
+    <row r="37" spans="1:14" ht="16.5" thickBot="1">
+      <c r="A37" s="29"/>
+      <c r="B37" s="30"/>
+      <c r="C37" s="31"/>
+      <c r="D37" s="31"/>
+      <c r="E37" s="32"/>
+      <c r="F37" s="31"/>
       <c r="K37" s="10"/>
       <c r="L37" s="11"/>
       <c r="M37" s="12"/>
@@ -1011,7 +1018,7 @@
       <c r="M38" s="12"/>
       <c r="N38" s="12"/>
     </row>
-    <row r="39" spans="1:14" ht="31.2" customHeight="1" thickBot="1">
+    <row r="39" spans="1:14" ht="31.15" customHeight="1" thickBot="1">
       <c r="A39" s="15"/>
       <c r="B39" s="14"/>
       <c r="C39" s="16"/>
@@ -1084,12 +1091,12 @@
       <c r="N44" s="12"/>
     </row>
     <row r="45" spans="1:14" ht="15.6" customHeight="1" thickBot="1">
-      <c r="A45" s="26"/>
-      <c r="B45" s="27"/>
-      <c r="C45" s="28"/>
-      <c r="D45" s="28"/>
-      <c r="E45" s="29"/>
-      <c r="F45" s="30"/>
+      <c r="A45" s="33"/>
+      <c r="B45" s="34"/>
+      <c r="C45" s="35"/>
+      <c r="D45" s="35"/>
+      <c r="E45" s="32"/>
+      <c r="F45" s="36"/>
       <c r="K45" s="10"/>
       <c r="L45" s="11"/>
       <c r="M45" s="12"/>
@@ -1107,7 +1114,7 @@
       <c r="M46" s="12"/>
       <c r="N46" s="12"/>
     </row>
-    <row r="47" spans="1:14" ht="31.2" customHeight="1" thickBot="1">
+    <row r="47" spans="1:14" ht="31.15" customHeight="1" thickBot="1">
       <c r="A47" s="15"/>
       <c r="B47" s="14"/>
       <c r="C47" s="16"/>
@@ -1180,12 +1187,12 @@
       <c r="N52" s="12"/>
     </row>
     <row r="53" spans="1:14" ht="15.6" customHeight="1" thickBot="1">
-      <c r="A53" s="26"/>
-      <c r="B53" s="27"/>
-      <c r="C53" s="28"/>
-      <c r="D53" s="28"/>
-      <c r="E53" s="29"/>
-      <c r="F53" s="30"/>
+      <c r="A53" s="33"/>
+      <c r="B53" s="34"/>
+      <c r="C53" s="35"/>
+      <c r="D53" s="35"/>
+      <c r="E53" s="32"/>
+      <c r="F53" s="36"/>
       <c r="K53" s="12"/>
       <c r="L53" s="11"/>
       <c r="M53" s="12"/>
@@ -1198,10 +1205,10 @@
       <c r="N54" s="12"/>
     </row>
     <row r="55" spans="1:14" ht="15.75" customHeight="1">
-      <c r="D55" s="25" t="s">
+      <c r="D55" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="E55" s="34">
+      <c r="E55" s="38">
         <f>SUM(E6:E53)</f>
         <v>0</v>
       </c>

</xml_diff>